<commit_message>
Update documentation, fix bug in preprocess step 3, add run options from env vars
</commit_message>
<xml_diff>
--- a/webapp/static/recapse_input_columns_needed.xlsx
+++ b/webapp/static/recapse_input_columns_needed.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qiqiao/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\UG3-UH3\UH3\API development\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C40D51FF-FD9E-F844-AB87-D8B4AFC9E6E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{874E3C86-5419-42F8-9DBE-D9B9D8EF4581}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="22920" windowHeight="13820" xr2:uid="{2B0B6F1F-FF0D-1B43-88F1-A09A08CD04AE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20520" windowHeight="12300" xr2:uid="{2B0B6F1F-FF0D-1B43-88F1-A09A08CD04AE}"/>
   </bookViews>
   <sheets>
     <sheet name="Columns_inputs" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="156">
   <si>
     <t>study_id</t>
   </si>
@@ -84,33 +84,6 @@
     <t>BN</t>
   </si>
   <si>
-    <t>C501</t>
-  </si>
-  <si>
-    <t>C502</t>
-  </si>
-  <si>
-    <t>C503</t>
-  </si>
-  <si>
-    <t>C504</t>
-  </si>
-  <si>
-    <t>C505</t>
-  </si>
-  <si>
-    <t>C506</t>
-  </si>
-  <si>
-    <t>C507</t>
-  </si>
-  <si>
-    <t>C508</t>
-  </si>
-  <si>
-    <t>C509</t>
-  </si>
-  <si>
     <t>site_o (first 6 will be used if more than 6 detected)</t>
   </si>
   <si>
@@ -150,9 +123,6 @@
     <t>Date_dx</t>
   </si>
   <si>
-    <t>Age</t>
-  </si>
-  <si>
     <t>Grade</t>
   </si>
   <si>
@@ -174,15 +144,6 @@
     <t>RXSummSurgPrimSite</t>
   </si>
   <si>
-    <t>radiation</t>
-  </si>
-  <si>
-    <t>chemo</t>
-  </si>
-  <si>
-    <t>hormone</t>
-  </si>
-  <si>
     <t>Year_Diag</t>
   </si>
   <si>
@@ -534,28 +495,23 @@
     <t>Claims_date</t>
   </si>
   <si>
-    <r>
-      <t>SEERSummStg2000</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> (note: it's better to call this varaible "SEERSummStg", as it's not just based on the 2000 version when generating the variable)</t>
-    </r>
-  </si>
-  <si>
-    <t>Medicare drug code observed in the claim file</t>
+    <t>Brand Name</t>
+  </si>
+  <si>
+    <t>Generic Name</t>
+  </si>
+  <si>
+    <t>review_1recur_dt</t>
+  </si>
+  <si>
+    <t>Date_1Recur</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -594,12 +550,6 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -699,7 +649,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -726,7 +676,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -737,7 +686,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1073,57 +1022,57 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49F64F08-3C42-094F-BBCD-5B2CE85EB79D}">
-  <dimension ref="A1:F52"/>
+  <dimension ref="A1:F48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8:F9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="41.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="41.5" customWidth="1"/>
     <col min="3" max="3" width="34" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="39" customWidth="1"/>
-    <col min="5" max="5" width="17.83203125" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.875" style="10" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="41.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="19" t="s">
-        <v>147</v>
-      </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="20" t="s">
-        <v>146</v>
-      </c>
-      <c r="D1" s="20"/>
-      <c r="E1" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="F1" s="21"/>
-    </row>
-    <row r="2" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="B1" s="18"/>
+      <c r="C1" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="D1" s="19"/>
+      <c r="E1" s="20" t="s">
+        <v>135</v>
+      </c>
+      <c r="F1" s="20"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>134</v>
+        <v>121</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>135</v>
+        <v>122</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
       <c r="E2" s="16" t="s">
         <v>9</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>0</v>
       </c>
@@ -1134,77 +1083,77 @@
         <v>2</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>157</v>
+        <v>144</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>15</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>26</v>
+        <v>120</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="22" t="s">
-        <v>152</v>
+      <c r="D4" s="21" t="s">
+        <v>139</v>
       </c>
       <c r="E4" s="13" t="s">
         <v>10</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>16</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>26</v>
+        <v>123</v>
       </c>
       <c r="C5" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="22"/>
+      <c r="D5" s="21"/>
       <c r="E5" s="13" t="s">
-        <v>160</v>
+        <v>147</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="12" t="s">
         <v>17</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="C6" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="22"/>
+      <c r="D6" s="21"/>
       <c r="E6" s="13" t="s">
         <v>12</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="12" t="s">
         <v>18</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>26</v>
+        <v>124</v>
       </c>
       <c r="C7" s="12" t="s">
         <v>6</v>
@@ -1216,15 +1165,15 @@
         <v>11</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>19</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="C8" s="12" t="s">
         <v>7</v>
@@ -1235,16 +1184,16 @@
       <c r="E8" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="F8" s="18" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="F8" s="12" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>20</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C9" s="12" t="s">
         <v>8</v>
@@ -1255,512 +1204,416 @@
       <c r="E9" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="F9" s="18" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="F9" s="12" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
         <v>21</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>153</v>
+        <v>140</v>
       </c>
       <c r="E10" s="13" t="s">
         <v>1</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>22</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>154</v>
+        <v>141</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
         <v>23</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="E12" s="13"/>
       <c r="F12" s="12"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
         <v>24</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>133</v>
+        <v>24</v>
       </c>
       <c r="C13" s="12"/>
       <c r="D13" s="12"/>
       <c r="E13" s="13"/>
       <c r="F13" s="12"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
         <v>25</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>136</v>
+        <v>25</v>
       </c>
       <c r="C14" s="12"/>
       <c r="D14" s="12"/>
       <c r="E14" s="13"/>
       <c r="F14" s="12"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
         <v>26</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>26</v>
+        <v>125</v>
       </c>
       <c r="C15" s="12"/>
       <c r="D15" s="12"/>
       <c r="E15" s="13"/>
       <c r="F15" s="12"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>27</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>137</v>
+        <v>27</v>
       </c>
       <c r="C16" s="12"/>
       <c r="D16" s="12"/>
       <c r="E16" s="13"/>
       <c r="F16" s="12"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>28</v>
+        <v>127</v>
       </c>
       <c r="C17" s="12"/>
       <c r="D17" s="12"/>
       <c r="E17" s="13"/>
       <c r="F17" s="12"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>29</v>
+        <v>128</v>
       </c>
       <c r="C18" s="12"/>
       <c r="D18" s="12"/>
       <c r="E18" s="13"/>
       <c r="F18" s="12"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C19" s="12"/>
       <c r="D19" s="12"/>
       <c r="E19" s="13"/>
       <c r="F19" s="12"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C20" s="12"/>
       <c r="D20" s="12"/>
       <c r="E20" s="13"/>
       <c r="F20" s="12"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>32</v>
+        <v>129</v>
       </c>
       <c r="C21" s="12"/>
       <c r="D21" s="12"/>
       <c r="E21" s="13"/>
       <c r="F21" s="12"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C22" s="12"/>
       <c r="D22" s="12"/>
       <c r="E22" s="13"/>
       <c r="F22" s="12"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C23" s="12"/>
       <c r="D23" s="12"/>
       <c r="E23" s="13"/>
       <c r="F23" s="12"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="12" t="s">
-        <v>35</v>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="13" t="s">
+        <v>130</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="C24" s="12"/>
       <c r="D24" s="12"/>
       <c r="E24" s="13"/>
       <c r="F24" s="12"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>36</v>
+        <v>131</v>
       </c>
       <c r="C25" s="12"/>
-      <c r="D25" s="12"/>
+      <c r="D25" s="9"/>
       <c r="E25" s="13"/>
-      <c r="F25" s="12"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F25" s="9"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="B26" s="9" t="s">
-        <v>139</v>
+        <v>38</v>
+      </c>
+      <c r="B26" s="12" t="s">
+        <v>38</v>
       </c>
       <c r="C26" s="12"/>
-      <c r="D26" s="9"/>
+      <c r="D26" s="12"/>
       <c r="E26" s="13"/>
-      <c r="F26" s="9"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F26" s="12"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>140</v>
+        <v>39</v>
       </c>
       <c r="C27" s="12"/>
       <c r="D27" s="12"/>
       <c r="E27" s="13"/>
       <c r="F27" s="12"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>141</v>
+        <v>40</v>
       </c>
       <c r="C28" s="12"/>
       <c r="D28" s="12"/>
       <c r="E28" s="13"/>
       <c r="F28" s="12"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C29" s="12"/>
       <c r="D29" s="12"/>
       <c r="E29" s="13"/>
       <c r="F29" s="12"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C30" s="12"/>
       <c r="D30" s="12"/>
       <c r="E30" s="13"/>
       <c r="F30" s="12"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>142</v>
+        <v>42</v>
       </c>
       <c r="C31" s="12"/>
       <c r="D31" s="12"/>
       <c r="E31" s="13"/>
       <c r="F31" s="12"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="B32" s="12" t="s">
-        <v>41</v>
+        <v>43</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>43</v>
       </c>
       <c r="C32" s="12"/>
       <c r="D32" s="12"/>
       <c r="E32" s="13"/>
       <c r="F32" s="12"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="B33" s="12" t="s">
-        <v>42</v>
+        <v>44</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>132</v>
       </c>
       <c r="C33" s="12"/>
       <c r="D33" s="12"/>
       <c r="E33" s="13"/>
       <c r="F33" s="12"/>
     </row>
-    <row r="34" spans="1:6" ht="68" x14ac:dyDescent="0.2">
-      <c r="A34" s="13" t="s">
-        <v>165</v>
-      </c>
-      <c r="B34" s="12" t="s">
-        <v>143</v>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>126</v>
       </c>
       <c r="C34" s="12"/>
       <c r="D34" s="12"/>
       <c r="E34" s="13"/>
       <c r="F34" s="12"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="B35" s="12" t="s">
-        <v>53</v>
+        <v>46</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>46</v>
       </c>
       <c r="C35" s="12"/>
       <c r="D35" s="12"/>
       <c r="E35" s="13"/>
       <c r="F35" s="12"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="12" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B36" s="12" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C36" s="12"/>
       <c r="D36" s="12"/>
       <c r="E36" s="13"/>
       <c r="F36" s="12"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A37" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="B37" s="12" t="s">
-        <v>52</v>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>154</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>155</v>
       </c>
       <c r="C37" s="12"/>
       <c r="D37" s="12"/>
       <c r="E37" s="13"/>
       <c r="F37" s="12"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A38" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="B38" s="12" t="s">
-        <v>144</v>
-      </c>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C38" s="12"/>
       <c r="D38" s="12"/>
       <c r="E38" s="13"/>
       <c r="F38" s="12"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A39" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="B39" s="12" t="s">
-        <v>51</v>
-      </c>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C39" s="12"/>
       <c r="D39" s="12"/>
       <c r="E39" s="13"/>
       <c r="F39" s="12"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A40" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="B40" s="12" t="s">
-        <v>52</v>
-      </c>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C40" s="12"/>
       <c r="D40" s="12"/>
       <c r="E40" s="13"/>
       <c r="F40" s="12"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A41" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="B41" s="12" t="s">
-        <v>53</v>
-      </c>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C41" s="12"/>
-      <c r="D41" s="12"/>
+      <c r="D41" s="9"/>
       <c r="E41" s="13"/>
-      <c r="F41" s="12"/>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A42" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="B42" s="12" t="s">
-        <v>44</v>
-      </c>
+      <c r="F41" s="9"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C42" s="12"/>
-      <c r="D42" s="12"/>
+      <c r="D42" s="9"/>
       <c r="E42" s="13"/>
-      <c r="F42" s="12"/>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A43" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="B43" s="12" t="s">
-        <v>54</v>
-      </c>
+      <c r="F42" s="9"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C43" s="12"/>
-      <c r="D43" s="12"/>
+      <c r="D43" s="9"/>
       <c r="E43" s="13"/>
-      <c r="F43" s="12"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A44" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="B44" s="12" t="s">
-        <v>55</v>
-      </c>
+      <c r="F43" s="9"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C44" s="12"/>
-      <c r="D44" s="12"/>
+      <c r="D44" s="9"/>
       <c r="E44" s="13"/>
-      <c r="F44" s="12"/>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A45" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="B45" s="9" t="s">
-        <v>56</v>
-      </c>
+      <c r="F44" s="9"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C45" s="12"/>
-      <c r="D45" s="9"/>
+      <c r="D45" s="12"/>
       <c r="E45" s="13"/>
-      <c r="F45" s="9"/>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A46" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="B46" s="9" t="s">
-        <v>145</v>
-      </c>
-      <c r="C46" s="12"/>
-      <c r="D46" s="9"/>
-      <c r="E46" s="13"/>
-      <c r="F46" s="9"/>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A47" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="B47" s="9" t="s">
-        <v>139</v>
-      </c>
-      <c r="C47" s="12"/>
-      <c r="D47" s="9"/>
-      <c r="E47" s="13"/>
-      <c r="F47" s="9"/>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A48" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="B48" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="C48" s="12"/>
-      <c r="D48" s="9"/>
-      <c r="E48" s="13"/>
-      <c r="F48" s="9"/>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A49" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="B49" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="C49" s="12"/>
-      <c r="D49" s="12"/>
-      <c r="E49" s="13"/>
-      <c r="F49" s="12"/>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="F52" s="12"/>
+      <c r="F45" s="12"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F48" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1782,447 +1635,447 @@
       <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="4" max="4" width="56.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="56.125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="109" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E20" s="3"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E21" s="3"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D22" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+      <c r="E22" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B23" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+      <c r="C23" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B24" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
+      <c r="C24" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D24" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
+      <c r="E24" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="D25" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="B9" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
+      <c r="E25" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="D26" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="B10" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="E20" s="3"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="E21" s="3"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="D22" s="8" t="s">
+      <c r="E26" s="3" t="s">
         <v>97</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="D24" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="D26" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>